<commit_message>
Complete Documentation. Still need to finish documentation for CourseInfo.py.
</commit_message>
<xml_diff>
--- a/Masterfile.xlsx
+++ b/Masterfile.xlsx
@@ -1,68 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Documents\GitHub\Tutor-Center-Login\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
-  <si>
-    <t>a01661687</t>
-  </si>
-  <si>
-    <t>Freshman</t>
-  </si>
-  <si>
-    <t>BENG 1000: Intro to Undergraduate Research</t>
-  </si>
-  <si>
-    <t>BENG</t>
-  </si>
-  <si>
-    <t>Tuesday,July 17,2018</t>
-  </si>
-  <si>
-    <t>Tuesday</t>
-  </si>
-  <si>
-    <t>BIEN</t>
-  </si>
-  <si>
-    <t>03:38 PM</t>
-  </si>
-  <si>
-    <t>03:39 PM</t>
-  </si>
-  <si>
-    <t>03:40 PM</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -78,15 +51,24 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -352,98 +334,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A2:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Explicitly directed to save to "Main Data" sheet.
</commit_message>
<xml_diff>
--- a/Masterfile.xlsx
+++ b/Masterfile.xlsx
@@ -1,31 +1,65 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Documents\GitHub\Tutor-Center-Login\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{957AF675-2A62-4AAB-AA78-80331949109A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Main Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>A-number</t>
+  </si>
+  <si>
+    <t>Class Rank</t>
+  </si>
+  <si>
+    <t>Major</t>
+  </si>
+  <si>
+    <t>Course Prefix</t>
+  </si>
+  <si>
+    <t>Course Name</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Time In</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -53,8 +87,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -334,23 +369,52 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="A2:H4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="41" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>